<commit_message>
update FR and NFR reuirements
</commit_message>
<xml_diff>
--- a/Project Requierments.xlsx
+++ b/Project Requierments.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
-  <si>
-    <t>requermets of place order - FR</t>
-  </si>
-  <si>
-    <t>requermets of place order - NFR</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+  <si>
+    <t>requirements of place order - FR</t>
+  </si>
+  <si>
+    <t>requirements of place order - NFR</t>
   </si>
   <si>
     <t>the system will allow remote connection</t>
@@ -91,52 +91,61 @@
     <t>after 2 hours the bill for the table is sent to the customer</t>
   </si>
   <si>
-    <t>the system will allow a customer to enter the waiting list if there isnt a free table</t>
+    <t xml:space="preserve">the system will allow a customer to enter the waiting list </t>
   </si>
   <si>
     <t>a customer can pay remotley or at a terminal</t>
   </si>
   <si>
-    <t>the system will be able to recognize if 15 minutes has been passed and the customer hasnt arrived</t>
+    <t>the system will be able to recognize how much time has been passed</t>
   </si>
   <si>
     <t>the bill for a member is reduced by 10%</t>
   </si>
   <si>
-    <t>the system will be able to send a new code if the cutomer lost his code</t>
+    <t>the system will be able to generate codes</t>
   </si>
   <si>
     <t>the table will be available immidieatly after payment</t>
   </si>
   <si>
-    <t xml:space="preserve">the ststem will be able to produce the bill after 2 hours of sitting </t>
+    <t xml:space="preserve">the ststem will be able to produce bills </t>
   </si>
   <si>
     <t>the information displayed</t>
   </si>
   <si>
-    <t>the system will be able to recognize a subscriber and give him a 10% discount</t>
+    <t>the system will be able to distinguish between customers types</t>
   </si>
   <si>
     <t>the system will be available 24/7 for future orders outside the resturant working hours</t>
   </si>
   <si>
-    <t xml:space="preserve">the system will enable the option for a subscriber to view his order history/visits.. </t>
+    <t xml:space="preserve">the system will enable more options for a subscriber  </t>
   </si>
   <si>
     <t>access for each interface will requaire verefication(subscriber/worker..)</t>
   </si>
   <si>
-    <t>the system will be able to change a table status(occupied/available)</t>
+    <t>the system will be able to change a table status</t>
   </si>
   <si>
     <t>it will not be possible to assign the same table to two customers simultaneosly</t>
   </si>
   <si>
-    <t xml:space="preserve">the system will be able to recognize a worker and will present to him the list/reservations/tables in real time </t>
-  </si>
-  <si>
     <t>all customers data will be stored securely</t>
+  </si>
+  <si>
+    <t>entry to the waiting list depends if there isnt a free table</t>
+  </si>
+  <si>
+    <t>if the cutomer lost his code the system will regenerate a new one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subscriber options are: view his order history/visits.. </t>
+  </si>
+  <si>
+    <t>table staus can be: occupied/available</t>
   </si>
 </sst>
 </file>
@@ -754,17 +763,44 @@
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="5">
-        <v>20.0</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="C23" s="5"/>
       <c r="I23" s="5">
         <v>20.0</v>
       </c>
       <c r="J23" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="I24" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="J24" s="5" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="I25" s="5">
+        <v>22.0</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="I26" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="I27" s="5">
+        <v>24.0</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>